<commit_message>
changes to engineering plan
</commit_message>
<xml_diff>
--- a/documents/Engineering Plan.xlsx
+++ b/documents/Engineering Plan.xlsx
@@ -283,6 +283,9 @@
       </filters>
     </filterColumn>
   </autoFilter>
+  <sortState ref="A2:E55">
+    <sortCondition ref="B1:B58"/>
+  </sortState>
   <tableColumns count="5">
     <tableColumn id="1" name="Feature/Workitem"/>
     <tableColumn id="2" name="Priority"/>
@@ -584,7 +587,7 @@
   <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,10 +616,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -630,7 +633,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -639,10 +642,10 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -664,16 +667,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -681,7 +684,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -690,10 +693,10 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -715,24 +718,24 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -741,15 +744,15 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E9">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -761,7 +764,7 @@
         <v>56</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -832,19 +835,19 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -860,7 +863,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -869,7 +872,7 @@
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E19">
         <v>8</v>
@@ -877,7 +880,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -886,7 +889,7 @@
         <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -894,7 +897,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -903,15 +906,15 @@
         <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E21">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -920,15 +923,15 @@
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E22">
-        <v>24</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -937,7 +940,7 @@
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E23">
         <v>8</v>
@@ -945,10 +948,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24" t="s">
         <v>10</v>
@@ -957,7 +960,7 @@
         <v>53</v>
       </c>
       <c r="E24">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -979,24 +982,24 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26" t="s">
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E26">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -1005,15 +1008,15 @@
         <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E27">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -1025,15 +1028,15 @@
         <v>53</v>
       </c>
       <c r="E28">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29" t="s">
         <v>10</v>
@@ -1041,13 +1044,13 @@
       <c r="D29" t="s">
         <v>56</v>
       </c>
-      <c r="E29">
-        <v>4</v>
+      <c r="E29" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -1059,12 +1062,12 @@
         <v>56</v>
       </c>
       <c r="E30">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -1076,12 +1079,12 @@
         <v>56</v>
       </c>
       <c r="E31">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -1090,7 +1093,7 @@
         <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E32">
         <v>2</v>
@@ -1115,7 +1118,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -1132,27 +1135,27 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C35" t="s">
         <v>10</v>
       </c>
       <c r="D35" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E35">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="B36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C36" t="s">
         <v>10</v>
@@ -1161,12 +1164,12 @@
         <v>56</v>
       </c>
       <c r="E36">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -1183,10 +1186,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C38" t="s">
         <v>10</v>
@@ -1195,7 +1198,7 @@
         <v>53</v>
       </c>
       <c r="E38">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -1245,19 +1248,19 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C42" t="s">
         <v>10</v>
       </c>
       <c r="D42" t="s">
-        <v>56</v>
-      </c>
-      <c r="E42" t="s">
-        <v>64</v>
+        <v>53</v>
+      </c>
+      <c r="E42">
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -1284,27 +1287,27 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C45" t="s">
         <v>10</v>
       </c>
       <c r="D45" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E45">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C46" t="s">
         <v>10</v>
@@ -1318,36 +1321,36 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C47" t="s">
         <v>10</v>
       </c>
       <c r="D47" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E47">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C48" t="s">
         <v>10</v>
       </c>
       <c r="D48" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E48">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -1386,27 +1389,27 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C51" t="s">
         <v>10</v>
       </c>
       <c r="D51" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E51">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C52" t="s">
         <v>10</v>
@@ -1420,16 +1423,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="B53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C53" t="s">
         <v>10</v>
       </c>
       <c r="D53" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E53">
         <v>4</v>

</xml_diff>